<commit_message>
Modified execl test file
</commit_message>
<xml_diff>
--- a/data/dev1/test.xlsx
+++ b/data/dev1/test.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -358,6 +358,21 @@
         <v>123</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>